<commit_message>
updated grades for 4, 5, 6 - good job!
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E702E28F-897D-4BA7-9017-1F1E7E3C52DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371279CF-1A6A-44F7-85D8-1374D5B1DFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="3315" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
   <si>
     <t>Student</t>
   </si>
@@ -60,7 +60,19 @@
     <t>Please read the comments in the cpp file I added</t>
   </si>
   <si>
-    <t>Only Created a sphere without code and didn’t create a room</t>
+    <t>4 UE</t>
+  </si>
+  <si>
+    <t>Good Job!</t>
+  </si>
+  <si>
+    <t>5 UE</t>
+  </si>
+  <si>
+    <t>6 UE</t>
+  </si>
+  <si>
+    <t>I Saw the fix</t>
   </si>
 </sst>
 </file>
@@ -431,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +479,11 @@
     <col min="26" max="26" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.42578125" style="3" customWidth="1"/>
     <col min="28" max="28" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="3"/>
+    <col min="29" max="40" width="15.85546875" style="3" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,8 +556,38 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -572,10 +615,10 @@
         <v>5</v>
       </c>
       <c r="K2" s="4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="4" t="s">
@@ -588,19 +631,49 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="4">
+        <v>100</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="4">
+        <v>100</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="Y2" s="5"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -629,8 +702,20 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -659,8 +744,20 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -689,8 +786,20 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -719,8 +828,20 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -749,8 +870,20 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -779,8 +912,20 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -809,8 +954,20 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -839,8 +996,20 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -869,8 +1038,20 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -899,8 +1080,20 @@
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="4"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -929,8 +1122,20 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="4"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -959,8 +1164,20 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="4"/>
+      <c r="AM14" s="4"/>
+      <c r="AN14" s="4"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -989,8 +1206,20 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="4"/>
+      <c r="AJ15" s="4"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="4"/>
+      <c r="AN15" s="4"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1019,8 +1248,20 @@
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="4"/>
+      <c r="AM16" s="4"/>
+      <c r="AN16" s="4"/>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1049,8 +1290,20 @@
       <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="4"/>
+      <c r="AN17" s="4"/>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1079,6 +1332,18 @@
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+      <c r="AN18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated grades for 4, 5 ,6. notice your class 5 folder is empty, you need to merge with main (check the README file on github). Also, for assignment 5 I gave you half the grade because you didnt implement another action
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846E735D-26A2-43D0-9E36-299013800FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BC8C17-A510-4716-9465-9E2D8E707149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2970" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Student</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>Very Good!</t>
+  </si>
+  <si>
+    <t>4 UE</t>
+  </si>
+  <si>
+    <t>Good Job!</t>
+  </si>
+  <si>
+    <t>5 UE</t>
+  </si>
+  <si>
+    <t>You didn’t implement a new action for shooting arrow 2</t>
+  </si>
+  <si>
+    <t>6 UE</t>
   </si>
 </sst>
 </file>
@@ -434,7 +449,7 @@
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -588,17 +603,35 @@
         <v>11</v>
       </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="4">
+        <v>100</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="4">
+        <v>50</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="Y2" s="5"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
+      <c r="Z2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>

</xml_diff>

<commit_message>
Updated grades for 4, 5, 6. you didnt implement a new action for arrow 2
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFF482A-CD43-4F91-8E4C-B02F7FF71CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF60B6A1-3C18-4A82-941F-A505AFAC7080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2970" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Student</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Mark Guriev</t>
+  </si>
+  <si>
+    <t>4 UE</t>
+  </si>
+  <si>
+    <t>Good Job!</t>
+  </si>
+  <si>
+    <t>5 UE</t>
+  </si>
+  <si>
+    <t>You didn’t implement a new action for shooting arrow 2</t>
+  </si>
+  <si>
+    <t>6 UE</t>
   </si>
 </sst>
 </file>
@@ -431,7 +446,7 @@
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD10"/>
+      <selection activeCell="R2" sqref="R2:AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +474,7 @@
     <col min="21" max="21" width="9.140625" style="3"/>
     <col min="22" max="22" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" style="3" customWidth="1"/>
     <col min="25" max="25" width="9.140625" style="3"/>
     <col min="26" max="26" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.42578125" style="3" customWidth="1"/>
@@ -541,7 +556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -585,17 +600,35 @@
         <v>9</v>
       </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="4">
+        <v>100</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="4">
+        <v>50</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="Y2" s="5"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
+      <c r="Z2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>

</xml_diff>

<commit_message>
updated grades on assignemtns 3-5
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9ED333-94AA-4AF0-918B-58319DB621AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C44E4D-EC97-4650-BF38-C88EAA3D5706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2970" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>Student</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>Great looking room! Amazing job!</t>
+  </si>
+  <si>
+    <t>3 CPP</t>
+  </si>
+  <si>
+    <t>See my comments  under the folder Shahar_Comments</t>
+  </si>
+  <si>
+    <t>Excellent!</t>
+  </si>
+  <si>
+    <t>4 UE</t>
+  </si>
+  <si>
+    <t>5 UE</t>
+  </si>
+  <si>
+    <t>did not create another actor type like Arrow and Target (see items 2 and 3 in class 5 HW)</t>
   </si>
 </sst>
 </file>
@@ -425,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AZ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +474,7 @@
     <col min="21" max="21" width="9.140625" style="3"/>
     <col min="22" max="22" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.28515625" style="3" customWidth="1"/>
     <col min="25" max="25" width="9.140625" style="3"/>
     <col min="26" max="26" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.42578125" style="3" customWidth="1"/>
@@ -464,7 +482,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,8 +555,68 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -572,23 +650,65 @@
         <v>9</v>
       </c>
       <c r="M2" s="5"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="4">
+        <v>75</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="4">
+        <v>100</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="4">
+        <v>33</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
+      <c r="AZ2" s="4"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -617,8 +737,32 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="5"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -647,8 +791,32 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
+      <c r="AZ4" s="4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -677,8 +845,32 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="4"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -707,8 +899,32 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -737,8 +953,32 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="4"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -767,8 +1007,32 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="4"/>
+      <c r="AY8" s="4"/>
+      <c r="AZ8" s="4"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -797,8 +1061,32 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
+      <c r="AR9" s="4"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="4"/>
+      <c r="AU9" s="4"/>
+      <c r="AV9" s="4"/>
+      <c r="AW9" s="5"/>
+      <c r="AX9" s="4"/>
+      <c r="AY9" s="4"/>
+      <c r="AZ9" s="4"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -827,8 +1115,32 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
+      <c r="AR10" s="4"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="4"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="4"/>
+      <c r="AY10" s="4"/>
+      <c r="AZ10" s="4"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -857,8 +1169,32 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="4"/>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="4"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="4"/>
+      <c r="AU11" s="4"/>
+      <c r="AV11" s="4"/>
+      <c r="AW11" s="5"/>
+      <c r="AX11" s="4"/>
+      <c r="AY11" s="4"/>
+      <c r="AZ11" s="4"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -887,8 +1223,32 @@
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="4"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="4"/>
+      <c r="AU12" s="4"/>
+      <c r="AV12" s="4"/>
+      <c r="AW12" s="5"/>
+      <c r="AX12" s="4"/>
+      <c r="AY12" s="4"/>
+      <c r="AZ12" s="4"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -917,6 +1277,30 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="4"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AS13" s="5"/>
+      <c r="AT13" s="4"/>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
+      <c r="AW13" s="5"/>
+      <c r="AX13" s="4"/>
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated grades for assignments 3-5
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66549BEB-57A6-4620-B5F6-20F90FBB901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A901C7-31AA-4F52-85EB-F926749E7666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6435" yWindow="5565" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
   <si>
     <t>Student</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>Nizar Lawen</t>
+  </si>
+  <si>
+    <t>3 CPP</t>
+  </si>
+  <si>
+    <t>Good!, see my comments</t>
+  </si>
+  <si>
+    <t>4 UE</t>
+  </si>
+  <si>
+    <t>5 UE</t>
+  </si>
+  <si>
+    <t>did not create another actor type like Arrow and Target (see items 2 and 3 in class 5 HW)</t>
   </si>
 </sst>
 </file>
@@ -425,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:BD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AS18" sqref="AS18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +471,7 @@
     <col min="21" max="21" width="9.140625" style="3"/>
     <col min="22" max="22" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5703125" style="3" customWidth="1"/>
     <col min="25" max="25" width="9.140625" style="3"/>
     <col min="26" max="26" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.42578125" style="3" customWidth="1"/>
@@ -464,7 +479,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,8 +552,78 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -572,23 +657,69 @@
         <v>8</v>
       </c>
       <c r="M2" s="5"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="4">
+        <v>80</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="4">
+        <v>100</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="4">
+        <v>33</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4"/>
+      <c r="BD2" s="4"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -617,8 +748,36 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="5"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
+      <c r="BA3" s="5"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4"/>
+      <c r="BD3" s="4"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -647,8 +806,36 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
+      <c r="AZ4" s="4"/>
+      <c r="BA4" s="5"/>
+      <c r="BB4" s="4"/>
+      <c r="BC4" s="4"/>
+      <c r="BD4" s="4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -677,8 +864,36 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="4"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="4"/>
+      <c r="BC5" s="4"/>
+      <c r="BD5" s="4"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -707,8 +922,36 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="5"/>
+      <c r="BB6" s="4"/>
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="4"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -737,8 +980,36 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="4"/>
+      <c r="BA7" s="5"/>
+      <c r="BB7" s="4"/>
+      <c r="BC7" s="4"/>
+      <c r="BD7" s="4"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -767,8 +1038,36 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="4"/>
+      <c r="AY8" s="4"/>
+      <c r="AZ8" s="4"/>
+      <c r="BA8" s="5"/>
+      <c r="BB8" s="4"/>
+      <c r="BC8" s="4"/>
+      <c r="BD8" s="4"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -797,8 +1096,36 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
+      <c r="AR9" s="4"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="4"/>
+      <c r="AU9" s="4"/>
+      <c r="AV9" s="4"/>
+      <c r="AW9" s="5"/>
+      <c r="AX9" s="4"/>
+      <c r="AY9" s="4"/>
+      <c r="AZ9" s="4"/>
+      <c r="BA9" s="5"/>
+      <c r="BB9" s="4"/>
+      <c r="BC9" s="4"/>
+      <c r="BD9" s="4"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -827,8 +1154,36 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
+      <c r="AR10" s="4"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="4"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="4"/>
+      <c r="AY10" s="4"/>
+      <c r="AZ10" s="4"/>
+      <c r="BA10" s="5"/>
+      <c r="BB10" s="4"/>
+      <c r="BC10" s="4"/>
+      <c r="BD10" s="4"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -857,6 +1212,34 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="4"/>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="4"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="4"/>
+      <c r="AU11" s="4"/>
+      <c r="AV11" s="4"/>
+      <c r="AW11" s="5"/>
+      <c r="AX11" s="4"/>
+      <c r="AY11" s="4"/>
+      <c r="AZ11" s="4"/>
+      <c r="BA11" s="5"/>
+      <c r="BB11" s="4"/>
+      <c r="BC11" s="4"/>
+      <c r="BD11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated grade for assignment 5 look in the excel - you are trying to bind OnCollision2 but your function name is OnCollision
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF60B6A1-3C18-4A82-941F-A505AFAC7080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374BA345-5740-4474-8003-BA6E112DB365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,10 +69,10 @@
     <t>5 UE</t>
   </si>
   <si>
-    <t>You didn’t implement a new action for shooting arrow 2</t>
-  </si>
-  <si>
     <t>6 UE</t>
+  </si>
+  <si>
+    <t>Great job except a small bug: You are binding the function "OnCollision2" when you do not have such a function</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:AB2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,14 +614,14 @@
         <v>13</v>
       </c>
       <c r="W2" s="4">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA2" s="4">
         <v>100</v>

</xml_diff>

<commit_message>
updated grade on HW5
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BC8C17-A510-4716-9465-9E2D8E707149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7010BE16-F1DA-4806-A7CA-62F8227F61D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,10 +72,10 @@
     <t>5 UE</t>
   </si>
   <si>
-    <t>You didn’t implement a new action for shooting arrow 2</t>
-  </si>
-  <si>
     <t>6 UE</t>
+  </si>
+  <si>
+    <t>You forgot to bind to a collision delegate in Arrow2's ctor</t>
   </si>
 </sst>
 </file>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -617,14 +617,14 @@
         <v>14</v>
       </c>
       <c r="W2" s="4">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA2" s="4">
         <v>100</v>

</xml_diff>

<commit_message>
Revert "Updated grade for assignment 5 look in the excel - you are trying to bind OnCollision2 but your function name is OnCollision"
This reverts commit 64d6dc9663b3c3a1f66533cbcbc723f8044a4ce4.
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374BA345-5740-4474-8003-BA6E112DB365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF60B6A1-3C18-4A82-941F-A505AFAC7080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,10 +69,10 @@
     <t>5 UE</t>
   </si>
   <si>
+    <t>You didn’t implement a new action for shooting arrow 2</t>
+  </si>
+  <si>
     <t>6 UE</t>
-  </si>
-  <si>
-    <t>Great job except a small bug: You are binding the function "OnCollision2" when you do not have such a function</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,14 +614,14 @@
         <v>13</v>
       </c>
       <c r="W2" s="4">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AA2" s="4">
         <v>100</v>

</xml_diff>

<commit_message>
Updated grades for HW 7
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEABFC9-F9DF-46E0-A4BD-03588EA97029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F5C72-1662-4B14-8008-9ED7722902A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2970" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>Student</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>not submitted</t>
+  </si>
+  <si>
+    <t>Not submitted</t>
+  </si>
+  <si>
+    <t>4 UE</t>
+  </si>
+  <si>
+    <t>5 UE</t>
+  </si>
+  <si>
+    <t>6 UE</t>
+  </si>
+  <si>
+    <t>7 CPP</t>
+  </si>
+  <si>
+    <t>my comments in the code</t>
   </si>
 </sst>
 </file>
@@ -428,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB16"/>
+  <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +485,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,12 +558,44 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
       <c r="C2" s="4">
         <v>100</v>
       </c>
@@ -579,19 +629,55 @@
         <v>8</v>
       </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="4">
+        <v>0</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="Y2" s="5"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>63</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -620,8 +706,20 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -650,8 +748,20 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -680,8 +790,20 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -710,8 +832,20 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -740,8 +874,20 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -770,8 +916,20 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -800,8 +958,20 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -830,8 +1000,20 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -860,8 +1042,20 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -890,8 +1084,20 @@
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="4"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -920,8 +1126,20 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="4"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -950,8 +1168,20 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="4"/>
+      <c r="AM14" s="4"/>
+      <c r="AN14" s="4"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -980,8 +1210,20 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="4"/>
+      <c r="AJ15" s="4"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="4"/>
+      <c r="AN15" s="4"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1010,6 +1252,18 @@
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="4"/>
+      <c r="AM16" s="4"/>
+      <c r="AN16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated grades, Very good job on HW 7, there is one issue (commas vs semi colons in vertex.cpp)
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC856C-0CFC-40DD-A655-7583F7F14597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602B7506-5C06-4422-B00D-B7AEBD33D8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2970" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>Student</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>did not create room with windows</t>
+  </si>
+  <si>
+    <t>4 UE</t>
+  </si>
+  <si>
+    <t>Not submitted</t>
+  </si>
+  <si>
+    <t>5 UE</t>
+  </si>
+  <si>
+    <t>6 UE</t>
+  </si>
+  <si>
+    <t>7 CPP</t>
+  </si>
+  <si>
+    <t>Very good!</t>
   </si>
 </sst>
 </file>
@@ -431,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +488,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,8 +561,18 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -588,19 +616,47 @@
         <v>8</v>
       </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="4">
+        <v>0</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="Y2" s="5"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>92</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -629,8 +685,12 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -659,8 +719,12 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -689,8 +753,12 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -719,8 +787,12 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -749,8 +821,12 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -779,8 +855,12 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -809,8 +889,12 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -839,8 +923,12 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -869,8 +957,12 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -899,8 +991,12 @@
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -929,8 +1025,12 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -959,6 +1059,10 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated grades up to 9 HW
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C44E4D-EC97-4650-BF38-C88EAA3D5706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C89EA3A-F5A4-4BB2-9AFA-99B3E4DE2B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>Student</t>
   </si>
@@ -60,9 +71,6 @@
     <t>3 CPP</t>
   </si>
   <si>
-    <t>See my comments  under the folder Shahar_Comments</t>
-  </si>
-  <si>
     <t>Excellent!</t>
   </si>
   <si>
@@ -72,7 +80,28 @@
     <t>5 UE</t>
   </si>
   <si>
-    <t>did not create another actor type like Arrow and Target (see items 2 and 3 in class 5 HW)</t>
+    <t>Saw the fix - excellent!</t>
+  </si>
+  <si>
+    <t>6 UE</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>7 CPP</t>
+  </si>
+  <si>
+    <t>see my comments</t>
+  </si>
+  <si>
+    <t>8 CPP</t>
+  </si>
+  <si>
+    <t>9 CPP</t>
+  </si>
+  <si>
+    <t>Excellent! (remember that 10 needs to be duplicated and not on the same solution)</t>
   </si>
 </sst>
 </file>
@@ -445,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +508,9 @@
     <col min="26" max="26" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.42578125" style="3" customWidth="1"/>
     <col min="28" max="28" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="3"/>
+    <col min="29" max="39" width="9.140625" style="3"/>
+    <col min="40" max="40" width="20" style="3" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="30" x14ac:dyDescent="0.25">
@@ -616,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -654,47 +685,71 @@
         <v>10</v>
       </c>
       <c r="O2" s="4">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S2" s="4">
         <v>100</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="4">
+        <v>100</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="4">
-        <v>33</v>
-      </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
+      <c r="AA2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AC2" s="5"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
+      <c r="AD2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>75</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="AG2" s="5"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
+      <c r="AH2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>99</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="AK2" s="5"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
+      <c r="AL2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="AO2" s="5"/>
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>

</xml_diff>

<commit_message>
updated grades up to HW 11, you need to separate between HW 9 and 10, otherwise 10 will get 0 grade
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7010BE16-F1DA-4806-A7CA-62F8227F61D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D63898-98C7-4CF9-8CAC-017010EBD3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>Student</t>
   </si>
@@ -76,6 +76,33 @@
   </si>
   <si>
     <t>You forgot to bind to a collision delegate in Arrow2's ctor</t>
+  </si>
+  <si>
+    <t>7 CPP</t>
+  </si>
+  <si>
+    <t>comments in the code</t>
+  </si>
+  <si>
+    <t>8 CPP</t>
+  </si>
+  <si>
+    <t>9 CPP</t>
+  </si>
+  <si>
+    <t>excellent</t>
+  </si>
+  <si>
+    <t>10 CPP</t>
+  </si>
+  <si>
+    <t>you need to submit this separately</t>
+  </si>
+  <si>
+    <t>11 CPP</t>
+  </si>
+  <si>
+    <t>very good, see my example in class 11 about the virtual Clone() method</t>
   </si>
 </sst>
 </file>
@@ -446,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AV17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:X2"/>
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +512,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,8 +585,58 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="105" x14ac:dyDescent="0.25">
+      <c r="AC1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV1" s="2"/>
+    </row>
+    <row r="2" spans="1:48" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -632,8 +709,58 @@
       <c r="AB2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>85</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT2" s="4">
+        <v>95</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AV2" s="5"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -663,7 +790,7 @@
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -693,7 +820,7 @@
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -723,7 +850,7 @@
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -753,7 +880,7 @@
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -783,7 +910,7 @@
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -813,7 +940,7 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -843,7 +970,7 @@
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -873,7 +1000,7 @@
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -903,7 +1030,7 @@
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -933,7 +1060,7 @@
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -963,7 +1090,7 @@
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -993,7 +1120,7 @@
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1023,7 +1150,7 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>

</xml_diff>

<commit_message>
Updated grades, Good Job!
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF60B6A1-3C18-4A82-941F-A505AFAC7080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A842027-5AC8-41B7-B460-F870D0AF8EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>Student</t>
   </si>
@@ -73,6 +73,36 @@
   </si>
   <si>
     <t>6 UE</t>
+  </si>
+  <si>
+    <t>7 CPP</t>
+  </si>
+  <si>
+    <t>Good!, Please read my comments</t>
+  </si>
+  <si>
+    <t>8 CPP</t>
+  </si>
+  <si>
+    <t>9 CPP</t>
+  </si>
+  <si>
+    <t>Excellent! (watch out for those memory leaks)</t>
+  </si>
+  <si>
+    <t>10 CPP</t>
+  </si>
+  <si>
+    <t>Very good!</t>
+  </si>
+  <si>
+    <t>11 CPP</t>
+  </si>
+  <si>
+    <t>See my Comments</t>
+  </si>
+  <si>
+    <t>12 CPP</t>
   </si>
 </sst>
 </file>
@@ -443,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:AB2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +512,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,8 +585,68 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -629,8 +719,68 @@
       <c r="AB2" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>85</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>99</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ2" s="4">
+        <v>91</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU2" s="4">
+        <v>71</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -659,8 +809,32 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="5"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -689,8 +863,32 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
+      <c r="AZ4" s="4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -719,8 +917,32 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="4"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -749,8 +971,32 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -779,8 +1025,32 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="4"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -809,8 +1079,32 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="4"/>
+      <c r="AY8" s="4"/>
+      <c r="AZ8" s="4"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -839,8 +1133,32 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
+      <c r="AR9" s="4"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="4"/>
+      <c r="AU9" s="4"/>
+      <c r="AV9" s="4"/>
+      <c r="AW9" s="5"/>
+      <c r="AX9" s="4"/>
+      <c r="AY9" s="4"/>
+      <c r="AZ9" s="4"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -869,8 +1187,32 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
+      <c r="AR10" s="4"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="4"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="4"/>
+      <c r="AY10" s="4"/>
+      <c r="AZ10" s="4"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -899,8 +1241,32 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="4"/>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="4"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="4"/>
+      <c r="AU11" s="4"/>
+      <c r="AV11" s="4"/>
+      <c r="AW11" s="5"/>
+      <c r="AX11" s="4"/>
+      <c r="AY11" s="4"/>
+      <c r="AZ11" s="4"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -929,6 +1295,30 @@
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="4"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="4"/>
+      <c r="AU12" s="4"/>
+      <c r="AV12" s="4"/>
+      <c r="AW12" s="5"/>
+      <c r="AX12" s="4"/>
+      <c r="AY12" s="4"/>
+      <c r="AZ12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated grade for Assignment 5
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A842027-5AC8-41B7-B460-F870D0AF8EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C6498B-3CCB-4E91-8587-6BAFD865CF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>Student</t>
   </si>
@@ -67,9 +78,6 @@
   </si>
   <si>
     <t>5 UE</t>
-  </si>
-  <si>
-    <t>You didn’t implement a new action for shooting arrow 2</t>
   </si>
   <si>
     <t>6 UE</t>
@@ -475,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AZ2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,14 +712,14 @@
         <v>13</v>
       </c>
       <c r="W2" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA2" s="4">
         <v>100</v>
@@ -721,17 +729,17 @@
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AE2" s="4">
         <v>85</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AG2" s="5"/>
       <c r="AH2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AI2" s="4">
         <v>100</v>
@@ -741,37 +749,37 @@
       </c>
       <c r="AK2" s="5"/>
       <c r="AL2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AM2" s="4">
         <v>99</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AO2" s="5"/>
       <c r="AP2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AQ2" s="4">
         <v>91</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AS2" s="5"/>
       <c r="AT2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AU2" s="4">
         <v>71</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AW2" s="5"/>
       <c r="AX2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AY2" s="4">
         <v>100</v>

</xml_diff>

<commit_message>
Updated grades, Very good job on assignment 12!
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD0477B-D0F6-4814-B017-FBE0F57EE679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44577E08-1059-45E2-91EB-FFE1D899C83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>Student</t>
   </si>
@@ -104,16 +104,10 @@
     <t>10 CPP</t>
   </si>
   <si>
-    <t>Very good!</t>
-  </si>
-  <si>
     <t>11 CPP</t>
   </si>
   <si>
     <t>12 CPP</t>
-  </si>
-  <si>
-    <t>Not submitted</t>
   </si>
 </sst>
 </file>
@@ -486,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2:AZ2"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2:AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,14 +761,14 @@
         <v>21</v>
       </c>
       <c r="AQ2" s="4">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="AS2" s="5"/>
       <c r="AT2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AU2" s="4">
         <v>100</v>
@@ -784,13 +778,13 @@
       </c>
       <c r="AW2" s="5"/>
       <c r="AX2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AY2" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated grade for final project - well done!
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF77984F-926D-4F55-B574-87B1CD4E034A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B2D233-B34D-4E83-9088-9CB2078328AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t>Student</t>
   </si>
@@ -67,9 +67,6 @@
     <t>3 CPP</t>
   </si>
   <si>
-    <t>Not submitted</t>
-  </si>
-  <si>
     <t>4 UE</t>
   </si>
   <si>
@@ -110,13 +107,19 @@
   </si>
   <si>
     <t>Saw the fix, see my comments</t>
+  </si>
+  <si>
+    <t>Final Project</t>
+  </si>
+  <si>
+    <t>Well done!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +135,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -199,6 +214,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:BA2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="BC5" sqref="BC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,37 +725,37 @@
         <v>100</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S2" s="4">
         <v>0</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W2" s="4">
         <v>0</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA2" s="4">
         <v>0</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="4" t="s">
@@ -751,63 +769,63 @@
       </c>
       <c r="AG2" s="5"/>
       <c r="AH2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI2" s="4">
         <v>100</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AK2" s="5"/>
       <c r="AL2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AM2" s="4">
         <v>100</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AO2" s="5"/>
       <c r="AP2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AQ2" s="4">
         <v>90</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AS2" s="5"/>
       <c r="AT2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AU2" s="4">
         <v>92</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AW2" s="5"/>
       <c r="AX2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AY2" s="4">
         <v>100</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BA2" s="2"/>
-      <c r="BB2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="BC2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>13</v>
+      <c r="BB2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="BC2" s="9">
+        <v>100</v>
+      </c>
+      <c r="BD2" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
@@ -1797,6 +1815,7 @@
       <c r="BD19" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated grades for final project
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_CPP_Course_2023_A\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD1DB30-1781-4C55-8258-D510D64B8B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507BA74E-3C96-4518-991C-92D837502D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
   <si>
     <t>Student</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>12 CPP</t>
+  </si>
+  <si>
+    <t>Final Project</t>
+  </si>
+  <si>
+    <t>Very Good!</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY18"/>
+  <dimension ref="A1:BD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2:AZ2"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2:BD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +524,7 @@
     <col min="41" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,8 +627,48 @@
       <c r="AN1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:51" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -725,32 +771,46 @@
       <c r="AN2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AQ2" s="3">
+      <c r="AQ2" s="4">
         <v>100</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AU2" s="3">
+      <c r="AU2" s="4">
         <v>100</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AV2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AY2" s="3">
+      <c r="AY2" s="4">
         <v>80</v>
       </c>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>90</v>
+      </c>
+      <c r="BD2" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -791,8 +851,24 @@
       <c r="AL3" s="4"/>
       <c r="AM3" s="4"/>
       <c r="AN3" s="4"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4"/>
+      <c r="BD3" s="4"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -833,8 +909,24 @@
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
+      <c r="AZ4" s="4"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="4"/>
+      <c r="BC4" s="4"/>
+      <c r="BD4" s="4"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -875,8 +967,24 @@
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="4"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="4"/>
+      <c r="BC5" s="4"/>
+      <c r="BD5" s="4"/>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -917,8 +1025,24 @@
       <c r="AL6" s="4"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="4"/>
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="4"/>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -959,8 +1083,24 @@
       <c r="AL7" s="4"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="4"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="4"/>
+      <c r="BC7" s="4"/>
+      <c r="BD7" s="4"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1001,8 +1141,24 @@
       <c r="AL8" s="4"/>
       <c r="AM8" s="4"/>
       <c r="AN8" s="4"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="4"/>
+      <c r="AY8" s="4"/>
+      <c r="AZ8" s="4"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="4"/>
+      <c r="BC8" s="4"/>
+      <c r="BD8" s="4"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1043,8 +1199,24 @@
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
+      <c r="AR9" s="4"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="4"/>
+      <c r="AU9" s="4"/>
+      <c r="AV9" s="4"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="4"/>
+      <c r="AY9" s="4"/>
+      <c r="AZ9" s="4"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="4"/>
+      <c r="BC9" s="4"/>
+      <c r="BD9" s="4"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1085,8 +1257,24 @@
       <c r="AL10" s="4"/>
       <c r="AM10" s="4"/>
       <c r="AN10" s="4"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
+      <c r="AR10" s="4"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="4"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="4"/>
+      <c r="AY10" s="4"/>
+      <c r="AZ10" s="4"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="4"/>
+      <c r="BC10" s="4"/>
+      <c r="BD10" s="4"/>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1127,8 +1315,24 @@
       <c r="AL11" s="4"/>
       <c r="AM11" s="4"/>
       <c r="AN11" s="4"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="4"/>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="4"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="4"/>
+      <c r="AU11" s="4"/>
+      <c r="AV11" s="4"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="4"/>
+      <c r="AY11" s="4"/>
+      <c r="AZ11" s="4"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="4"/>
+      <c r="BC11" s="4"/>
+      <c r="BD11" s="4"/>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1169,8 +1373,24 @@
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="4"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="4"/>
+      <c r="AU12" s="4"/>
+      <c r="AV12" s="4"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="4"/>
+      <c r="AY12" s="4"/>
+      <c r="AZ12" s="4"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="4"/>
+      <c r="BC12" s="4"/>
+      <c r="BD12" s="4"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1211,8 +1431,24 @@
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="4"/>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="4"/>
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="4"/>
+      <c r="BA13" s="2"/>
+      <c r="BB13" s="4"/>
+      <c r="BC13" s="4"/>
+      <c r="BD13" s="4"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1253,8 +1489,24 @@
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="4"/>
+      <c r="AQ14" s="4"/>
+      <c r="AR14" s="4"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="4"/>
+      <c r="AU14" s="4"/>
+      <c r="AV14" s="4"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="4"/>
+      <c r="AY14" s="4"/>
+      <c r="AZ14" s="4"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="4"/>
+      <c r="BC14" s="4"/>
+      <c r="BD14" s="4"/>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1295,8 +1547,24 @@
       <c r="AL15" s="4"/>
       <c r="AM15" s="4"/>
       <c r="AN15" s="4"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="4"/>
+      <c r="AQ15" s="4"/>
+      <c r="AR15" s="4"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="4"/>
+      <c r="AU15" s="4"/>
+      <c r="AV15" s="4"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="4"/>
+      <c r="AY15" s="4"/>
+      <c r="AZ15" s="4"/>
+      <c r="BA15" s="2"/>
+      <c r="BB15" s="4"/>
+      <c r="BC15" s="4"/>
+      <c r="BD15" s="4"/>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1337,8 +1605,24 @@
       <c r="AL16" s="4"/>
       <c r="AM16" s="4"/>
       <c r="AN16" s="4"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="4"/>
+      <c r="AQ16" s="4"/>
+      <c r="AR16" s="4"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="4"/>
+      <c r="AU16" s="4"/>
+      <c r="AV16" s="4"/>
+      <c r="AW16" s="2"/>
+      <c r="AX16" s="4"/>
+      <c r="AY16" s="4"/>
+      <c r="AZ16" s="4"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="4"/>
+      <c r="BC16" s="4"/>
+      <c r="BD16" s="4"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1379,8 +1663,24 @@
       <c r="AL17" s="4"/>
       <c r="AM17" s="4"/>
       <c r="AN17" s="4"/>
+      <c r="AO17" s="2"/>
+      <c r="AP17" s="4"/>
+      <c r="AQ17" s="4"/>
+      <c r="AR17" s="4"/>
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="4"/>
+      <c r="AU17" s="4"/>
+      <c r="AV17" s="4"/>
+      <c r="AW17" s="2"/>
+      <c r="AX17" s="4"/>
+      <c r="AY17" s="4"/>
+      <c r="AZ17" s="4"/>
+      <c r="BA17" s="2"/>
+      <c r="BB17" s="4"/>
+      <c r="BC17" s="4"/>
+      <c r="BD17" s="4"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1421,6 +1721,22 @@
       <c r="AL18" s="4"/>
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
+      <c r="AO18" s="2"/>
+      <c r="AP18" s="4"/>
+      <c r="AQ18" s="4"/>
+      <c r="AR18" s="4"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="4"/>
+      <c r="AU18" s="4"/>
+      <c r="AV18" s="4"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="4"/>
+      <c r="AY18" s="4"/>
+      <c r="AZ18" s="4"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="4"/>
+      <c r="BC18" s="4"/>
+      <c r="BD18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated final project grade
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_CPP_Course_2023_A\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0134BD17-994F-4073-AF3D-29C01DE98BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF4ECE-EC6D-416C-B4E7-720FABA1FDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
   <si>
     <t>Student</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Final Project</t>
-  </si>
-  <si>
-    <t>Didn't make at least 20 dialogs, and 2 conditional…</t>
   </si>
 </sst>
 </file>
@@ -479,7 +476,7 @@
   <dimension ref="A1:BD8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AT14" sqref="AT14"/>
+      <selection activeCell="BC2" sqref="BC2:BD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -797,10 +794,10 @@
         <v>25</v>
       </c>
       <c r="BC2" s="4">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated grade for final project
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_CPP_Course_2023_A\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CA764F-C15F-4FDD-9697-3A3DD3953400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C859F48D-E288-4D36-A652-16498D424CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
   <si>
     <t>Student</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>your code didn’t compile - I wrote the mistakes in the comments folder</t>
+  </si>
+  <si>
+    <t>Final Project</t>
   </si>
 </sst>
 </file>
@@ -480,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="BA2" sqref="BA2:BD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,9 +798,15 @@
         <v>8</v>
       </c>
       <c r="BA2" s="5"/>
-      <c r="BB2" s="4"/>
-      <c r="BC2" s="4"/>
-      <c r="BD2" s="4"/>
+      <c r="BB2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>90</v>
+      </c>
+      <c r="BD2" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>

</xml_diff>

<commit_message>
Updated grades and final project grade
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_UnrealEngineCourse\Grades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_CPP_Course_2023_A\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF24DB64-A260-4446-BD95-F647606397A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EF87BA-29DC-4D26-8B94-D408C0E24D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>Student</t>
   </si>
@@ -73,6 +73,33 @@
   </si>
   <si>
     <t>7 CPP</t>
+  </si>
+  <si>
+    <t>Very good!</t>
+  </si>
+  <si>
+    <t>8 CPP</t>
+  </si>
+  <si>
+    <t>9 CPP</t>
+  </si>
+  <si>
+    <t>10 CPP</t>
+  </si>
+  <si>
+    <t>Very good! (didn’t implement copy assignment operator properly - not copying values)</t>
+  </si>
+  <si>
+    <t>11 CPP</t>
+  </si>
+  <si>
+    <t>Very good (read my comments)</t>
+  </si>
+  <si>
+    <t>12 CPP</t>
+  </si>
+  <si>
+    <t>Final Project</t>
   </si>
 </sst>
 </file>
@@ -443,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:BD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF2"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="BA1" sqref="BA1:BA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +509,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,8 +582,78 @@
       <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -627,14 +724,78 @@
       <c r="AB2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AE2" s="3">
-        <v>0</v>
+      <c r="AE2" s="4">
+        <v>90</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ2" s="4">
+        <v>90</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU2" s="4">
+        <v>90</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>100</v>
+      </c>
+      <c r="BD2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -663,8 +824,36 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4"/>
+      <c r="BD3" s="4"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -693,8 +882,36 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
+      <c r="AZ4" s="4"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="4"/>
+      <c r="BC4" s="4"/>
+      <c r="BD4" s="4"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -723,8 +940,36 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="4"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="4"/>
+      <c r="BC5" s="4"/>
+      <c r="BD5" s="4"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -753,6 +998,34 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="4"/>
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated grades - Moed bet
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiltan\Tiltan_CPP_Course_2023_A\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F77B5F-A5B3-4EC6-A840-83A3CC2BEBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867E5752-08AC-4127-8018-66062E90F9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="23">
   <si>
     <t>Student</t>
   </si>
@@ -484,7 +484,7 @@
   <dimension ref="A1:BD19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2:BD2"/>
+      <selection activeCell="BC3" sqref="BC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,41 +712,33 @@
         <v>11</v>
       </c>
       <c r="S2" s="4">
-        <v>0</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="T2" s="4"/>
       <c r="U2" s="5"/>
       <c r="V2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="W2" s="4">
-        <v>0</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="X2" s="4"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="AA2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="AB2" s="4"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AE2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="AF2" s="4"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="4" t="s">
         <v>15</v>
@@ -762,11 +754,9 @@
         <v>17</v>
       </c>
       <c r="AM2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="AN2" s="4"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="4" t="s">
         <v>18</v>
@@ -802,7 +792,7 @@
         <v>21</v>
       </c>
       <c r="BC2" s="4">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="BD2" s="4" t="s">
         <v>22</v>

</xml_diff>